<commit_message>
added: ppd lab5 without karatsuba
</commit_message>
<xml_diff>
--- a/RPA/Dispatcher/Dispatcher/Data/Input/InputFile.xlsx
+++ b/RPA/Dispatcher/Dispatcher/Data/Input/InputFile.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Desktop\Managed Services\UBB Mentorship\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Desktop\folders\UniversityThirdYear\RPA\Dispatcher\Dispatcher\Data\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB4A0B5B-B853-46ED-AF35-2EE38B110439}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA909953-AD17-4C93-8710-BE8EC477D118}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2244" yWindow="2040" windowWidth="17280" windowHeight="9960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="41">
   <si>
     <t>Bucuresti</t>
   </si>
@@ -43,9 +43,6 @@
     <t>F</t>
   </si>
   <si>
-    <t>Barba</t>
-  </si>
-  <si>
     <t>Cluj</t>
   </si>
   <si>
@@ -67,15 +64,9 @@
     <t>Bistrita</t>
   </si>
   <si>
-    <t>Masaj barbati</t>
-  </si>
-  <si>
     <t>Sibiu</t>
   </si>
   <si>
-    <t>Targu-Mures</t>
-  </si>
-  <si>
     <t>Coafat</t>
   </si>
   <si>
@@ -152,6 +143,12 @@
   </si>
   <si>
     <t>Service type</t>
+  </si>
+  <si>
+    <t>Targu Mures</t>
+  </si>
+  <si>
+    <t>Masaj</t>
   </si>
 </sst>
 </file>
@@ -472,28 +469,28 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.33203125" customWidth="1"/>
+    <col min="1" max="1" width="24.28515625" customWidth="1"/>
     <col min="2" max="2" width="28" customWidth="1"/>
-    <col min="3" max="3" width="24.6640625" customWidth="1"/>
+    <col min="3" max="3" width="24.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -504,7 +501,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -512,95 +509,95 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
         <v>8</v>
       </c>
-      <c r="C5" t="s">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
         <v>10</v>
       </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C11" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -617,42 +614,42 @@
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" customWidth="1"/>
-    <col min="2" max="2" width="20.5546875" customWidth="1"/>
-    <col min="3" max="3" width="14.44140625" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" customWidth="1"/>
-    <col min="5" max="5" width="13.44140625" customWidth="1"/>
-    <col min="6" max="6" width="18.88671875" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" customWidth="1"/>
+    <col min="2" max="2" width="20.5703125" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>23</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
         <v>24</v>
-      </c>
-      <c r="C1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" t="s">
-        <v>27</v>
       </c>
       <c r="C2">
         <v>5</v>
@@ -664,12 +661,12 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="F2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C3">
         <v>5</v>
@@ -681,12 +678,12 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="F3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C4">
         <v>5</v>
@@ -698,12 +695,12 @@
         <v>4.7</v>
       </c>
       <c r="F4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C5">
         <v>5</v>
@@ -715,12 +712,12 @@
         <v>5</v>
       </c>
       <c r="F5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
-        <v>33</v>
       </c>
       <c r="C6">
         <v>5</v>
@@ -732,12 +729,12 @@
         <v>4.7</v>
       </c>
       <c r="F6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C7">
         <v>4.9000000000000004</v>
@@ -749,12 +746,12 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="F7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C8">
         <v>5</v>
@@ -766,12 +763,12 @@
         <v>4.7</v>
       </c>
       <c r="F8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C9">
         <v>5</v>
@@ -783,12 +780,12 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="F9" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C10">
         <v>5</v>
@@ -800,12 +797,12 @@
         <v>4.8</v>
       </c>
       <c r="F10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C11">
         <v>5</v>
@@ -817,7 +814,7 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="F11" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added: ppd lab 5
</commit_message>
<xml_diff>
--- a/RPA/Dispatcher/Dispatcher/Data/Input/InputFile.xlsx
+++ b/RPA/Dispatcher/Dispatcher/Data/Input/InputFile.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Desktop\folders\UniversityThirdYear\RPA\Dispatcher\Dispatcher\Data\Input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Desktop\Managed Services\UBB Mentorship\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA909953-AD17-4C93-8710-BE8EC477D118}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB4A0B5B-B853-46ED-AF35-2EE38B110439}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2244" yWindow="2040" windowWidth="17280" windowHeight="9960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="42">
   <si>
     <t>Bucuresti</t>
   </si>
@@ -43,6 +43,9 @@
     <t>F</t>
   </si>
   <si>
+    <t>Barba</t>
+  </si>
+  <si>
     <t>Cluj</t>
   </si>
   <si>
@@ -64,9 +67,15 @@
     <t>Bistrita</t>
   </si>
   <si>
+    <t>Masaj barbati</t>
+  </si>
+  <si>
     <t>Sibiu</t>
   </si>
   <si>
+    <t>Targu-Mures</t>
+  </si>
+  <si>
     <t>Coafat</t>
   </si>
   <si>
@@ -143,12 +152,6 @@
   </si>
   <si>
     <t>Service type</t>
-  </si>
-  <si>
-    <t>Targu Mures</t>
-  </si>
-  <si>
-    <t>Masaj</t>
   </si>
 </sst>
 </file>
@@ -469,28 +472,28 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.28515625" customWidth="1"/>
+    <col min="1" max="1" width="24.33203125" customWidth="1"/>
     <col min="2" max="2" width="28" customWidth="1"/>
-    <col min="3" max="3" width="24.7109375" customWidth="1"/>
+    <col min="3" max="3" width="24.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -501,7 +504,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -509,95 +512,95 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" t="s">
-        <v>7</v>
-      </c>
       <c r="C6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -614,42 +617,42 @@
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" customWidth="1"/>
-    <col min="2" max="2" width="20.5703125" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" customWidth="1"/>
-    <col min="6" max="6" width="18.85546875" customWidth="1"/>
+    <col min="1" max="1" width="10.88671875" customWidth="1"/>
+    <col min="2" max="2" width="20.5546875" customWidth="1"/>
+    <col min="3" max="3" width="14.44140625" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" customWidth="1"/>
+    <col min="5" max="5" width="13.44140625" customWidth="1"/>
+    <col min="6" max="6" width="18.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" t="s">
         <v>21</v>
       </c>
-      <c r="C1" t="s">
-        <v>18</v>
-      </c>
       <c r="D1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="E1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C2">
         <v>5</v>
@@ -661,12 +664,12 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="F2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C3">
         <v>5</v>
@@ -678,12 +681,12 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="F3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C4">
         <v>5</v>
@@ -695,12 +698,12 @@
         <v>4.7</v>
       </c>
       <c r="F4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C5">
         <v>5</v>
@@ -712,12 +715,12 @@
         <v>5</v>
       </c>
       <c r="F5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C6">
         <v>5</v>
@@ -729,12 +732,12 @@
         <v>4.7</v>
       </c>
       <c r="F6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C7">
         <v>4.9000000000000004</v>
@@ -746,12 +749,12 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="F7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C8">
         <v>5</v>
@@ -763,12 +766,12 @@
         <v>4.7</v>
       </c>
       <c r="F8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C9">
         <v>5</v>
@@ -780,12 +783,12 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="F9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C10">
         <v>5</v>
@@ -797,12 +800,12 @@
         <v>4.8</v>
       </c>
       <c r="F10" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C11">
         <v>5</v>
@@ -814,7 +817,7 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="F11" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added: rpa input file and exception in case of no data is found
</commit_message>
<xml_diff>
--- a/RPA/Dispatcher/Dispatcher/Data/Input/InputFile.xlsx
+++ b/RPA/Dispatcher/Dispatcher/Data/Input/InputFile.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Desktop\Managed Services\UBB Mentorship\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Desktop\folders\UniversityThirdYear\RPA\Dispatcher\Dispatcher\Data\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB4A0B5B-B853-46ED-AF35-2EE38B110439}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B922A306-ADCD-4580-AB79-2C00F6E9915E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2244" yWindow="2040" windowWidth="17280" windowHeight="9960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="1" r:id="rId1"/>
@@ -26,69 +26,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="42">
-  <si>
-    <t>Bucuresti</t>
-  </si>
-  <si>
-    <t>Manichiura &amp; Pedichiura</t>
-  </si>
-  <si>
-    <t>Iasi</t>
-  </si>
-  <si>
-    <t>M</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
   <si>
     <t>F</t>
   </si>
   <si>
-    <t>Barba</t>
-  </si>
-  <si>
-    <t>Cluj</t>
-  </si>
-  <si>
-    <t>Tuns</t>
-  </si>
-  <si>
-    <t>Timisoara</t>
-  </si>
-  <si>
-    <t>Gene</t>
-  </si>
-  <si>
-    <t xml:space="preserve">F </t>
-  </si>
-  <si>
-    <t>Epilare definitiva</t>
-  </si>
-  <si>
-    <t>Bistrita</t>
-  </si>
-  <si>
-    <t>Masaj barbati</t>
-  </si>
-  <si>
-    <t>Sibiu</t>
-  </si>
-  <si>
-    <t>Targu-Mures</t>
-  </si>
-  <si>
-    <t>Coafat</t>
-  </si>
-  <si>
     <t>Zalau</t>
   </si>
   <si>
     <t>Vopsit</t>
-  </si>
-  <si>
-    <t>Satu Mare</t>
-  </si>
-  <si>
-    <t>Pensat</t>
   </si>
   <si>
     <t>Rating Stailer</t>
@@ -469,138 +415,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.33203125" customWidth="1"/>
+    <col min="1" max="1" width="24.28515625" customWidth="1"/>
     <col min="2" max="2" width="28" customWidth="1"/>
-    <col min="3" max="3" width="24.6640625" customWidth="1"/>
+    <col min="3" max="3" width="24.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
         <v>23</v>
       </c>
-      <c r="C1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
         <v>2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>3</v>
-      </c>
-      <c r="B11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -617,42 +464,42 @@
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" customWidth="1"/>
-    <col min="2" max="2" width="20.5546875" customWidth="1"/>
-    <col min="3" max="3" width="14.44140625" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" customWidth="1"/>
-    <col min="5" max="5" width="13.44140625" customWidth="1"/>
-    <col min="6" max="6" width="18.88671875" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" customWidth="1"/>
+    <col min="2" max="2" width="20.5703125" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
         <v>21</v>
       </c>
-      <c r="D1" t="s">
-        <v>39</v>
-      </c>
       <c r="E1" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="C2">
         <v>5</v>
@@ -664,12 +511,12 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="F2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="C3">
         <v>5</v>
@@ -681,12 +528,12 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="F3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="C4">
         <v>5</v>
@@ -698,12 +545,12 @@
         <v>4.7</v>
       </c>
       <c r="F4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="C5">
         <v>5</v>
@@ -715,12 +562,12 @@
         <v>5</v>
       </c>
       <c r="F5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="C6">
         <v>5</v>
@@ -732,12 +579,12 @@
         <v>4.7</v>
       </c>
       <c r="F6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="C7">
         <v>4.9000000000000004</v>
@@ -749,12 +596,12 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="F7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="C8">
         <v>5</v>
@@ -766,12 +613,12 @@
         <v>4.7</v>
       </c>
       <c r="F8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="C9">
         <v>5</v>
@@ -783,12 +630,12 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="F9" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="C10">
         <v>5</v>
@@ -800,12 +647,12 @@
         <v>4.8</v>
       </c>
       <c r="F10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="C11">
         <v>5</v>
@@ -817,7 +664,7 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="F11" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>